<commit_message>
Ajeitando a regressão básica
</commit_message>
<xml_diff>
--- a/documentacao/P&I/Plano de Homologação.xlsx
+++ b/documentacao/P&I/Plano de Homologação.xlsx
@@ -1,58 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\sdpiar\sdpiar\documentacao\P&amp;I\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEC532B-0DA8-4DDF-B06D-E9307088952F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{375F5880-ABFA-4414-8D00-245EBB4A2157}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="1" r:id="rId1"/>
     <sheet name="Cenários" sheetId="2" r:id="rId2"/>
     <sheet name="Regrassão Básica" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="124">
+  <si>
+    <t>Projeto:</t>
+  </si>
   <si>
     <t>SDPIAR</t>
   </si>
   <si>
+    <t>Código da demanda:</t>
+  </si>
+  <si>
+    <t>Usuários Envolvidos:</t>
+  </si>
+  <si>
     <t>Fernando Brandão</t>
   </si>
   <si>
     <t>Analistas Envolvidos:</t>
   </si>
   <si>
-    <t>Usuários Envolvidos:</t>
-  </si>
-  <si>
-    <t>Código da demanda:</t>
-  </si>
-  <si>
-    <t>Projeto:</t>
+    <t>A Gente</t>
   </si>
   <si>
     <t>Data da Homologação:</t>
   </si>
   <si>
-    <t>A Gente</t>
-  </si>
-  <si>
     <t>Premissas</t>
   </si>
   <si>
@@ -62,6 +68,9 @@
     <t>Entregável</t>
   </si>
   <si>
+    <t>Critério de Aceitação</t>
+  </si>
+  <si>
     <t>Resposável</t>
   </si>
   <si>
@@ -71,12 +80,27 @@
     <t>Status em Homologação</t>
   </si>
   <si>
-    <t>Critério de Aceitação</t>
+    <t>Cadastro de Usuários</t>
+  </si>
+  <si>
+    <t>Permitir o cadastro de vários usuários no sistema.</t>
   </si>
   <si>
     <t>Anderson</t>
   </si>
   <si>
+    <t>Login de Usuários</t>
+  </si>
+  <si>
+    <t>Permitir o login de vários usuários no sistema.</t>
+  </si>
+  <si>
+    <t>Dashboard e gráficos</t>
+  </si>
+  <si>
+    <t>Painel de monitoramento com gráficos e indicadores de temperatura e umidade.</t>
+  </si>
+  <si>
     <t>ID da Funcionalidade</t>
   </si>
   <si>
@@ -92,75 +116,57 @@
     <t>Prioridade</t>
   </si>
   <si>
+    <t>RF001-01</t>
+  </si>
+  <si>
+    <t>Permitir o cadastro do usuário no sistema utilizando Usuário, Senha, Nome, Data de Nascimento, RG, Sexo, Endereço, CEP, Telefone e Email.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação dos campos + botão(Cadastro) para cadastrar o usuário no sistema.</t>
+  </si>
+  <si>
+    <t>Usuário será cadastrado e redirecionado para a página de Login</t>
+  </si>
+  <si>
+    <t>RF001-02</t>
+  </si>
+  <si>
+    <t>Consistir os campos do "Cadastro" com dados válidos</t>
+  </si>
+  <si>
+    <t>Permitir a digitação nos campos do cadastro (Dados válidos)  para cadastrar o usuário no sistema.</t>
+  </si>
+  <si>
+    <t>Validar os dados inseridos nos campos. Se houver algum erro, exibir um alerta para o usuário</t>
+  </si>
+  <si>
     <t>RF002-01</t>
   </si>
   <si>
+    <t>Permitir o login do usuário utilizando "Usuário" e "Senha".</t>
+  </si>
+  <si>
+    <t>Permitir a digitação nos campos de Login + botão para autenticar o usuário no sistema.</t>
+  </si>
+  <si>
+    <t>Usuário será autenticado e redirecionado para a página com o dashboard e os gráficos</t>
+  </si>
+  <si>
     <t>RF002-02</t>
   </si>
   <si>
-    <t>Cadastro de Usuários</t>
-  </si>
-  <si>
-    <t>Login de Usuários</t>
-  </si>
-  <si>
-    <t>Dashboard e gráficos</t>
+    <t>Consistir os campos do "Login" com dados válidos.</t>
+  </si>
+  <si>
+    <t>Permitir a digitação nos campos de Login (Dados válidos) + botão para autenticar o usuário no sistema.</t>
+  </si>
+  <si>
+    <t>Válidar os dados inseridos nos campos. Se houver algum erro, exibir um alerta para o usuário.</t>
   </si>
   <si>
     <t>RF003-01</t>
   </si>
   <si>
-    <t>RF001-01</t>
-  </si>
-  <si>
-    <t>Permitir o cadastro do usuário no sistema utilizando Usuário, Senha, Nome, Data de Nascimento, RG, Sexo, Endereço, CEP, Telefone e Email.</t>
-  </si>
-  <si>
-    <t>Permitir a digitação dos campos + botão(Cadastro) para cadastrar o usuário no sistema.</t>
-  </si>
-  <si>
-    <t>Usuário será cadastrado e redirecionado para a página de Login</t>
-  </si>
-  <si>
-    <t>RF001-02</t>
-  </si>
-  <si>
-    <t>Consistir os campos do "Cadastro" com dados válidos</t>
-  </si>
-  <si>
-    <t>Validar os dados inseridos nos campos. Se houver algum erro, exibir um alerta para o usuário</t>
-  </si>
-  <si>
-    <t>Permitir o login do usuário utilizando "Usuário" e "Senha".</t>
-  </si>
-  <si>
-    <t>Permitir a digitação nos campos do cadastro (Dados válidos)  para cadastrar o usuário no sistema.</t>
-  </si>
-  <si>
-    <t>Permitir a digitação nos campos de Login + botão para autenticar o usuário no sistema.</t>
-  </si>
-  <si>
-    <t>Usuário será autenticado e redirecionado para a página com o dashboard e os gráficos</t>
-  </si>
-  <si>
-    <t>Consistir os campos do "Login" com dados válidos.</t>
-  </si>
-  <si>
-    <t>Permitir a digitação nos campos de Login (Dados válidos) + botão para autenticar o usuário no sistema.</t>
-  </si>
-  <si>
-    <t>Válidar os dados inseridos nos campos. Se houver algum erro, exibir um alerta para o usuário.</t>
-  </si>
-  <si>
-    <t>Painel de monitoramento com gráficos e indicadores de temperatura e umidade.</t>
-  </si>
-  <si>
-    <t>Permitir o login de vários usuários no sistema.</t>
-  </si>
-  <si>
-    <t>Permitir o cadastro de vários usuários no sistema.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Página consistindo de um painel de monitoramento e graficos com as médias de temperatura e umidade e indicadores de temp. e umid. </t>
   </si>
   <si>
@@ -170,18 +176,33 @@
     <t>Os dados devem vir em "tempo real" para que o usuário tenha a informação exata do que esta acontecendo.</t>
   </si>
   <si>
+    <t>RF003-02</t>
+  </si>
+  <si>
+    <t>Página consistindo de um campo para o cadastro de uma área nova.</t>
+  </si>
+  <si>
+    <t>Permitir o cadastro de uma área utilizando os sensores</t>
+  </si>
+  <si>
+    <t>Códigode Demanda:</t>
+  </si>
+  <si>
     <t>XXXX</t>
   </si>
   <si>
+    <t>Analista:</t>
+  </si>
+  <si>
+    <t>Wilma</t>
+  </si>
+  <si>
+    <t>Data:</t>
+  </si>
+  <si>
     <t>Versão:</t>
   </si>
   <si>
-    <t>Códigode Demanda:</t>
-  </si>
-  <si>
-    <t>Data:</t>
-  </si>
-  <si>
     <t>Objetos</t>
   </si>
   <si>
@@ -191,18 +212,21 @@
     <t>login.js</t>
   </si>
   <si>
+    <t>public/login.js</t>
+  </si>
+  <si>
+    <t>grafico.html/leituras.js</t>
+  </si>
+  <si>
+    <t>public/grafico.html</t>
+  </si>
+  <si>
     <t>Caso de Teste</t>
   </si>
   <si>
     <t>Testar o login do usuário</t>
   </si>
   <si>
-    <t>Analista:</t>
-  </si>
-  <si>
-    <t>public/login.js</t>
-  </si>
-  <si>
     <t>ID do TC</t>
   </si>
   <si>
@@ -215,36 +239,36 @@
     <t>Massa de Teste</t>
   </si>
   <si>
+    <t>Esperado / Valor esperado</t>
+  </si>
+  <si>
+    <t>Print Screen da tela esperada</t>
+  </si>
+  <si>
+    <t>Status - Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Status - Qualidade</t>
+  </si>
+  <si>
+    <t>PrintScreen de Evidência</t>
+  </si>
+  <si>
+    <t>RF002-01 - TC01</t>
+  </si>
+  <si>
+    <t>Abrir o site sdpiar.azurewebsites.net, selecionar a opção de Login; digitar o login do usuário no campo "Usuário"; ir para o campo de senha</t>
+  </si>
+  <si>
     <t>Login do usuário = Wilma123</t>
   </si>
   <si>
-    <t>Abrir o site sdpiar.azurewebsites.net, selecionar a opção de Login; digitar o login do usuário no campo "Usuário"; ir para o campo de senha</t>
-  </si>
-  <si>
     <t>Permitir sair do campo "Usuário" sem mensagem de erro</t>
   </si>
   <si>
-    <t>Esperado / Valor esperado</t>
-  </si>
-  <si>
-    <t>Print Screen da tela esperada</t>
-  </si>
-  <si>
-    <t>Status - Desenvolvimento</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>Status - Qualidade</t>
-  </si>
-  <si>
-    <t>PrintScreen de Evidência</t>
-  </si>
-  <si>
-    <t>RF002-01 - TC01</t>
-  </si>
-  <si>
     <t>RF002-01 - TC02</t>
   </si>
   <si>
@@ -266,12 +290,18 @@
     <t>Buscar no banco de dados o login do usuário</t>
   </si>
   <si>
+    <t>Usuário = Correto;                Senha = Correto;</t>
+  </si>
+  <si>
     <t>Permitir o login do usuário no sistema</t>
   </si>
   <si>
     <t>RF002-02 - TC04</t>
   </si>
   <si>
+    <t>Usuário = Correto;               Senha = Incorreto;</t>
+  </si>
+  <si>
     <t>Exibir a mensagem de erro "Usuário ou senha incorretos"</t>
   </si>
   <si>
@@ -281,7 +311,31 @@
     <t>Usuário = Incorreto;            Senha = Incorreto;</t>
   </si>
   <si>
-    <t>Usuário = Correto;                Senha = Correto;</t>
+    <t>RF003-01 - TC06</t>
+  </si>
+  <si>
+    <t>Página consistindo de um painel de monitoramento e graficos com as médias de temperatura e umidade e indicadores de temp. e umid.</t>
+  </si>
+  <si>
+    <t>Página com dashboards comunicando com a nuvem e recebendo os dados de temperatura e umidade</t>
+  </si>
+  <si>
+    <t>Ligar o arduino com o sensor;</t>
+  </si>
+  <si>
+    <t>Dashboards recebendo os dados de temperatura e umidade sem interrupções</t>
+  </si>
+  <si>
+    <t>RF003-02 - TC07</t>
+  </si>
+  <si>
+    <t>Cadastrar uma área para o usuário utilizando 3 sensores</t>
+  </si>
+  <si>
+    <t>Se o usuário tentar cadastrar um área utilizando apenas 2 sensores</t>
+  </si>
+  <si>
+    <t>Exibir uma mensagem de erro "Utilize 3 sensores para cadastrar a sua área"</t>
   </si>
   <si>
     <t>ID</t>
@@ -290,10 +344,19 @@
     <t>Descrição</t>
   </si>
   <si>
+    <t>Quando Fazer?</t>
+  </si>
+  <si>
     <t>Entrar no Site</t>
   </si>
   <si>
-    <t>Entrar no site www.meuprojeto.com</t>
+    <t>sdpiar.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>Fazer Sempre</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
   <si>
     <t>Login</t>
@@ -317,6 +380,12 @@
     <t>Verificar se os sensores exibidos são do usuário logado</t>
   </si>
   <si>
+    <t>Verificar se a área do usuário esta funcionando</t>
+  </si>
+  <si>
+    <t>Verificar se as notificações estão funcionando</t>
+  </si>
+  <si>
     <t>Logout</t>
   </si>
   <si>
@@ -329,12 +398,6 @@
     <t>Voltar para página principal do Site</t>
   </si>
   <si>
-    <t>Quando Fazer?</t>
-  </si>
-  <si>
-    <t>Fazer Sempre</t>
-  </si>
-  <si>
     <t>Teste Unitário:</t>
   </si>
   <si>
@@ -342,54 +405,6 @@
   </si>
   <si>
     <t>Status:</t>
-  </si>
-  <si>
-    <t>RF003-02</t>
-  </si>
-  <si>
-    <t>Página consistindo de um campo para o cadastro de uma área nova.</t>
-  </si>
-  <si>
-    <t>Permitir o cadastro de uma área utilizando os sensores</t>
-  </si>
-  <si>
-    <t>RF003-01 - TC06</t>
-  </si>
-  <si>
-    <t>Página consistindo de um painel de monitoramento e graficos com as médias de temperatura e umidade e indicadores de temp. e umid.</t>
-  </si>
-  <si>
-    <t>Página com dashboards comunicando com a nuvem e recebendo os dados de temperatura e umidade</t>
-  </si>
-  <si>
-    <t>Usuário = Correto;               Senha = Incorreto;</t>
-  </si>
-  <si>
-    <t>Ligar o arduino com o sensor;</t>
-  </si>
-  <si>
-    <t>Dashboards recebendo os dados de temperatura e umidade sem interrupções</t>
-  </si>
-  <si>
-    <t>RF003-02 - TC07</t>
-  </si>
-  <si>
-    <t>Cadastrar uma área para o usuário utilizando 3 sensores</t>
-  </si>
-  <si>
-    <t>Se o usuário tentar cadastrar um área utilizando apenas 2 sensores</t>
-  </si>
-  <si>
-    <t>Exibir uma mensagem de erro "Utilize 3 sensores para cadastrar a sua área"</t>
-  </si>
-  <si>
-    <t>Wilma</t>
-  </si>
-  <si>
-    <t>public/grafico.html</t>
-  </si>
-  <si>
-    <t>grafico.html/leituras.js</t>
   </si>
 </sst>
 </file>
@@ -399,7 +414,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,7 +677,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -689,26 +704,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,20 +725,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -743,8 +761,8 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1042,178 +1060,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:Q64"/>
   <sheetViews>
-    <sheetView topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59:G64"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E59" sqref="E53:G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D3" s="18" t="s">
+    <row r="3" spans="3:16">
+      <c r="D3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="3:16">
+      <c r="D4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="3:16">
+      <c r="D5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="3:16">
+      <c r="D6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="15" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="3:16">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="16">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="19">
         <v>43620</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="21" t="s">
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="9" spans="3:16">
+      <c r="C9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="3:16" ht="15" customHeight="1">
+      <c r="C10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="10" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="13"/>
-      <c r="M10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="3:16">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="3:16">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="3:16">
       <c r="C13" s="9">
         <v>1</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="K13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12">
+      <c r="K13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="21">
         <v>43609</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8"/>
@@ -1222,14 +1240,14 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
@@ -1238,40 +1256,40 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:16">
       <c r="C16" s="9">
         <v>2</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12">
+      <c r="K16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21">
         <v>43609</v>
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:17">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -1280,14 +1298,14 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:17">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
@@ -1296,38 +1314,38 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
-    <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:17" ht="15" customHeight="1">
       <c r="C19" s="9">
         <v>3</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12">
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="21">
         <v>43609</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="21"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:17">
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="8"/>
@@ -1336,14 +1354,14 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:17">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -1352,14 +1370,14 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:17">
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
@@ -1368,14 +1386,14 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:17">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1391,70 +1409,70 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q26" s="10"/>
-    </row>
-    <row r="27" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-    </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-    </row>
-    <row r="29" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17">
+      <c r="C26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q26" s="11"/>
+    </row>
+    <row r="27" spans="3:17" ht="15" customHeight="1">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+    </row>
+    <row r="28" spans="3:17">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+    </row>
+    <row r="29" spans="3:17" ht="15" customHeight="1">
       <c r="C29" s="9" t="s">
         <v>27</v>
       </c>
@@ -1479,7 +1497,7 @@
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:17">
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
@@ -1496,7 +1514,7 @@
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:17">
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
@@ -1513,7 +1531,7 @@
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
     </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:17">
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="8"/>
@@ -1530,7 +1548,7 @@
       <c r="P32" s="8"/>
       <c r="Q32" s="8"/>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:17">
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
@@ -1547,7 +1565,7 @@
       <c r="P33" s="8"/>
       <c r="Q33" s="8"/>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:17">
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
@@ -1564,7 +1582,7 @@
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
     </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:17">
       <c r="C35" s="9" t="s">
         <v>31</v>
       </c>
@@ -1575,12 +1593,12 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
@@ -1589,7 +1607,7 @@
       <c r="P35" s="8"/>
       <c r="Q35" s="8"/>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17">
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -1606,7 +1624,7 @@
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:17">
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="8"/>
@@ -1623,7 +1641,7 @@
       <c r="P37" s="8"/>
       <c r="Q37" s="8"/>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17">
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="8"/>
@@ -1640,7 +1658,7 @@
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
     </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:17">
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
@@ -1657,7 +1675,7 @@
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17">
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
@@ -1674,23 +1692,23 @@
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:17">
       <c r="C41" s="9" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
@@ -1699,7 +1717,7 @@
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
     </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:17">
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="8"/>
@@ -1716,7 +1734,7 @@
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17">
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="8"/>
@@ -1733,7 +1751,7 @@
       <c r="P43" s="8"/>
       <c r="Q43" s="8"/>
     </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17">
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="8"/>
@@ -1750,7 +1768,7 @@
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17">
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
@@ -1767,7 +1785,7 @@
       <c r="P45" s="8"/>
       <c r="Q45" s="8"/>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17">
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
@@ -1784,23 +1802,23 @@
       <c r="P46" s="8"/>
       <c r="Q46" s="8"/>
     </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17">
       <c r="C47" s="9" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
@@ -1809,7 +1827,7 @@
       <c r="P47" s="8"/>
       <c r="Q47" s="8"/>
     </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:17">
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
@@ -1826,7 +1844,7 @@
       <c r="P48" s="8"/>
       <c r="Q48" s="8"/>
     </row>
-    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:17">
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
@@ -1843,7 +1861,7 @@
       <c r="P49" s="8"/>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:17">
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="8"/>
@@ -1860,7 +1878,7 @@
       <c r="P50" s="8"/>
       <c r="Q50" s="8"/>
     </row>
-    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:17">
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
@@ -1877,7 +1895,7 @@
       <c r="P51" s="8"/>
       <c r="Q51" s="8"/>
     </row>
-    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:17">
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
@@ -1894,9 +1912,9 @@
       <c r="P52" s="8"/>
       <c r="Q52" s="8"/>
     </row>
-    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:17">
       <c r="C53" s="9" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="8" t="s">
@@ -1919,7 +1937,7 @@
       <c r="P53" s="8"/>
       <c r="Q53" s="8"/>
     </row>
-    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:17">
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="8"/>
@@ -1936,7 +1954,7 @@
       <c r="P54" s="8"/>
       <c r="Q54" s="8"/>
     </row>
-    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:17">
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="8"/>
@@ -1953,7 +1971,7 @@
       <c r="P55" s="8"/>
       <c r="Q55" s="8"/>
     </row>
-    <row r="56" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:17">
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="8"/>
@@ -1970,7 +1988,7 @@
       <c r="P56" s="8"/>
       <c r="Q56" s="8"/>
     </row>
-    <row r="57" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:17">
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
@@ -1987,7 +2005,7 @@
       <c r="P57" s="8"/>
       <c r="Q57" s="8"/>
     </row>
-    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:17">
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
@@ -2004,18 +2022,18 @@
       <c r="P58" s="8"/>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:17">
       <c r="C59" s="9" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="8" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="I59" s="8"/>
       <c r="J59" s="8"/>
@@ -2029,7 +2047,7 @@
       <c r="P59" s="8"/>
       <c r="Q59" s="8"/>
     </row>
-    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:17">
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="8"/>
@@ -2046,7 +2064,7 @@
       <c r="P60" s="8"/>
       <c r="Q60" s="8"/>
     </row>
-    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:17">
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="8"/>
@@ -2063,7 +2081,7 @@
       <c r="P61" s="8"/>
       <c r="Q61" s="8"/>
     </row>
-    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:17">
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="8"/>
@@ -2080,7 +2098,7 @@
       <c r="P62" s="8"/>
       <c r="Q62" s="8"/>
     </row>
-    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:17">
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
@@ -2097,7 +2115,7 @@
       <c r="P63" s="8"/>
       <c r="Q63" s="8"/>
     </row>
-    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:17">
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
@@ -2116,12 +2134,61 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="P59:Q64"/>
-    <mergeCell ref="C59:D64"/>
-    <mergeCell ref="E59:G64"/>
-    <mergeCell ref="H59:J64"/>
-    <mergeCell ref="K59:M64"/>
-    <mergeCell ref="N59:O64"/>
+    <mergeCell ref="P29:Q34"/>
+    <mergeCell ref="E29:G34"/>
+    <mergeCell ref="C29:D34"/>
+    <mergeCell ref="H29:J34"/>
+    <mergeCell ref="K29:M34"/>
+    <mergeCell ref="N29:O34"/>
+    <mergeCell ref="P26:Q28"/>
+    <mergeCell ref="C16:D18"/>
+    <mergeCell ref="E16:G18"/>
+    <mergeCell ref="H16:J18"/>
+    <mergeCell ref="K16:L18"/>
+    <mergeCell ref="H19:J22"/>
+    <mergeCell ref="E19:G22"/>
+    <mergeCell ref="C41:D46"/>
+    <mergeCell ref="E41:G46"/>
+    <mergeCell ref="H41:J46"/>
+    <mergeCell ref="M10:N12"/>
+    <mergeCell ref="E13:G15"/>
+    <mergeCell ref="C13:D15"/>
+    <mergeCell ref="K13:L15"/>
+    <mergeCell ref="M13:N15"/>
+    <mergeCell ref="C19:D22"/>
+    <mergeCell ref="K19:L22"/>
+    <mergeCell ref="C10:D12"/>
+    <mergeCell ref="E10:G12"/>
+    <mergeCell ref="H10:J12"/>
+    <mergeCell ref="K10:L12"/>
+    <mergeCell ref="M16:N18"/>
+    <mergeCell ref="M19:N22"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="O10:P12"/>
+    <mergeCell ref="H13:J15"/>
+    <mergeCell ref="C35:D40"/>
+    <mergeCell ref="E35:G40"/>
+    <mergeCell ref="H35:J40"/>
+    <mergeCell ref="K35:M40"/>
+    <mergeCell ref="N35:O40"/>
+    <mergeCell ref="O13:P15"/>
+    <mergeCell ref="P35:Q40"/>
+    <mergeCell ref="O16:P18"/>
+    <mergeCell ref="O19:P22"/>
+    <mergeCell ref="C26:D28"/>
+    <mergeCell ref="E26:G28"/>
+    <mergeCell ref="H26:J28"/>
+    <mergeCell ref="K26:M28"/>
+    <mergeCell ref="N26:O28"/>
     <mergeCell ref="P53:Q58"/>
     <mergeCell ref="C9:P9"/>
     <mergeCell ref="C53:D58"/>
@@ -2138,61 +2205,12 @@
     <mergeCell ref="K47:M52"/>
     <mergeCell ref="N47:O52"/>
     <mergeCell ref="P47:Q52"/>
-    <mergeCell ref="O10:P12"/>
-    <mergeCell ref="H13:J15"/>
-    <mergeCell ref="C35:D40"/>
-    <mergeCell ref="E35:G40"/>
-    <mergeCell ref="H35:J40"/>
-    <mergeCell ref="K35:M40"/>
-    <mergeCell ref="N35:O40"/>
-    <mergeCell ref="O13:P15"/>
-    <mergeCell ref="P35:Q40"/>
-    <mergeCell ref="O16:P18"/>
-    <mergeCell ref="O19:P22"/>
-    <mergeCell ref="C26:D28"/>
-    <mergeCell ref="E26:G28"/>
-    <mergeCell ref="H26:J28"/>
-    <mergeCell ref="K26:M28"/>
-    <mergeCell ref="N26:O28"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="C41:D46"/>
-    <mergeCell ref="E41:G46"/>
-    <mergeCell ref="H41:J46"/>
-    <mergeCell ref="M10:N12"/>
-    <mergeCell ref="E13:G15"/>
-    <mergeCell ref="C13:D15"/>
-    <mergeCell ref="K13:L15"/>
-    <mergeCell ref="M13:N15"/>
-    <mergeCell ref="C19:D22"/>
-    <mergeCell ref="K19:L22"/>
-    <mergeCell ref="C10:D12"/>
-    <mergeCell ref="E10:G12"/>
-    <mergeCell ref="H10:J12"/>
-    <mergeCell ref="K10:L12"/>
-    <mergeCell ref="M16:N18"/>
-    <mergeCell ref="M19:N22"/>
-    <mergeCell ref="P26:Q28"/>
-    <mergeCell ref="C16:D18"/>
-    <mergeCell ref="E16:G18"/>
-    <mergeCell ref="H16:J18"/>
-    <mergeCell ref="K16:L18"/>
-    <mergeCell ref="H19:J22"/>
-    <mergeCell ref="E19:G22"/>
-    <mergeCell ref="P29:Q34"/>
-    <mergeCell ref="E29:G34"/>
-    <mergeCell ref="C29:D34"/>
-    <mergeCell ref="H29:J34"/>
-    <mergeCell ref="K29:M34"/>
-    <mergeCell ref="N29:O34"/>
+    <mergeCell ref="P59:Q64"/>
+    <mergeCell ref="C59:D64"/>
+    <mergeCell ref="E59:G64"/>
+    <mergeCell ref="H59:J64"/>
+    <mergeCell ref="K59:M64"/>
+    <mergeCell ref="N59:O64"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2202,237 +2220,237 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+    <row r="2" spans="2:8">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23">
+        <v>43621</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="28">
-        <v>43621</v>
-      </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25">
-        <v>1</v>
-      </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="2:8">
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27">
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22" t="s">
+    <row r="18" spans="2:27">
+      <c r="B18" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22" t="s">
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22" t="s">
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22" t="s">
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="22" t="s">
+      <c r="Q18" s="26"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="22"/>
-      <c r="AA19" s="22"/>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="W18" s="26"/>
+      <c r="X18" s="26"/>
+      <c r="Y18" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="26"/>
+    </row>
+    <row r="19" spans="2:27">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="26"/>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="26"/>
+      <c r="AA19" s="26"/>
+    </row>
+    <row r="20" spans="2:27">
       <c r="B20" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
@@ -2440,12 +2458,12 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
       <c r="V20" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W20" s="8"/>
       <c r="X20" s="8"/>
@@ -2453,7 +2471,7 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="8"/>
@@ -2481,7 +2499,7 @@
       <c r="Z21" s="8"/>
       <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="8"/>
@@ -2509,7 +2527,7 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="8"/>
@@ -2537,7 +2555,7 @@
       <c r="Z23" s="8"/>
       <c r="AA23" s="8"/>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="8"/>
@@ -2565,7 +2583,7 @@
       <c r="Z24" s="8"/>
       <c r="AA24" s="8"/>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
@@ -2593,28 +2611,28 @@
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27">
       <c r="B26" s="9" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
@@ -2622,12 +2640,12 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
       <c r="S26" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
       <c r="V26" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W26" s="8"/>
       <c r="X26" s="8"/>
@@ -2635,7 +2653,7 @@
       <c r="Z26" s="8"/>
       <c r="AA26" s="8"/>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27">
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="8"/>
@@ -2663,7 +2681,7 @@
       <c r="Z27" s="8"/>
       <c r="AA27" s="8"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="8"/>
@@ -2691,7 +2709,7 @@
       <c r="Z28" s="8"/>
       <c r="AA28" s="8"/>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="8"/>
@@ -2719,7 +2737,7 @@
       <c r="Z29" s="8"/>
       <c r="AA29" s="8"/>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="8"/>
@@ -2747,7 +2765,7 @@
       <c r="Z30" s="8"/>
       <c r="AA30" s="8"/>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="8"/>
@@ -2775,28 +2793,28 @@
       <c r="Z31" s="8"/>
       <c r="AA31" s="8"/>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27">
       <c r="B32" s="9" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="8" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
@@ -2804,12 +2822,12 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
       <c r="V32" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W32" s="8"/>
       <c r="X32" s="8"/>
@@ -2817,7 +2835,7 @@
       <c r="Z32" s="8"/>
       <c r="AA32" s="8"/>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27">
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="8"/>
@@ -2845,7 +2863,7 @@
       <c r="Z33" s="8"/>
       <c r="AA33" s="8"/>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27">
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="8"/>
@@ -2873,7 +2891,7 @@
       <c r="Z34" s="8"/>
       <c r="AA34" s="8"/>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="8"/>
@@ -2901,7 +2919,7 @@
       <c r="Z35" s="8"/>
       <c r="AA35" s="8"/>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27">
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="8"/>
@@ -2929,7 +2947,7 @@
       <c r="Z36" s="8"/>
       <c r="AA36" s="8"/>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27">
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="8"/>
@@ -2957,28 +2975,28 @@
       <c r="Z37" s="8"/>
       <c r="AA37" s="8"/>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:27">
       <c r="B38" s="9" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="8" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
@@ -2986,12 +3004,12 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T38" s="8"/>
       <c r="U38" s="8"/>
       <c r="V38" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W38" s="8"/>
       <c r="X38" s="8"/>
@@ -2999,7 +3017,7 @@
       <c r="Z38" s="8"/>
       <c r="AA38" s="8"/>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:27">
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="8"/>
@@ -3027,7 +3045,7 @@
       <c r="Z39" s="8"/>
       <c r="AA39" s="8"/>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:27">
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="8"/>
@@ -3055,7 +3073,7 @@
       <c r="Z40" s="8"/>
       <c r="AA40" s="8"/>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:27">
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="8"/>
@@ -3083,7 +3101,7 @@
       <c r="Z41" s="8"/>
       <c r="AA41" s="8"/>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:27">
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="8"/>
@@ -3111,7 +3129,7 @@
       <c r="Z42" s="8"/>
       <c r="AA42" s="8"/>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:27">
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="8"/>
@@ -3139,28 +3157,28 @@
       <c r="Z43" s="8"/>
       <c r="AA43" s="8"/>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:27">
       <c r="B44" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="8" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
@@ -3168,12 +3186,12 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
       <c r="S44" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T44" s="8"/>
       <c r="U44" s="8"/>
       <c r="V44" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W44" s="8"/>
       <c r="X44" s="8"/>
@@ -3181,7 +3199,7 @@
       <c r="Z44" s="8"/>
       <c r="AA44" s="8"/>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:27">
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="8"/>
@@ -3209,7 +3227,7 @@
       <c r="Z45" s="8"/>
       <c r="AA45" s="8"/>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:27">
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="8"/>
@@ -3237,7 +3255,7 @@
       <c r="Z46" s="8"/>
       <c r="AA46" s="8"/>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:27">
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="8"/>
@@ -3265,7 +3283,7 @@
       <c r="Z47" s="8"/>
       <c r="AA47" s="8"/>
     </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:27">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="8"/>
@@ -3293,7 +3311,7 @@
       <c r="Z48" s="8"/>
       <c r="AA48" s="8"/>
     </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:27">
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="8"/>
@@ -3321,28 +3339,28 @@
       <c r="Z49" s="8"/>
       <c r="AA49" s="8"/>
     </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:27">
       <c r="B50" s="9" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="8" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="N50" s="8"/>
       <c r="O50" s="8"/>
@@ -3350,12 +3368,12 @@
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
       <c r="S50" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T50" s="8"/>
       <c r="U50" s="8"/>
       <c r="V50" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W50" s="8"/>
       <c r="X50" s="8"/>
@@ -3363,7 +3381,7 @@
       <c r="Z50" s="8"/>
       <c r="AA50" s="8"/>
     </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:27">
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="8"/>
@@ -3391,7 +3409,7 @@
       <c r="Z51" s="8"/>
       <c r="AA51" s="8"/>
     </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:27">
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="8"/>
@@ -3419,7 +3437,7 @@
       <c r="Z52" s="8"/>
       <c r="AA52" s="8"/>
     </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:27">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="8"/>
@@ -3447,7 +3465,7 @@
       <c r="Z53" s="8"/>
       <c r="AA53" s="8"/>
     </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:27">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="8"/>
@@ -3475,7 +3493,7 @@
       <c r="Z54" s="8"/>
       <c r="AA54" s="8"/>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:27">
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="8"/>
@@ -3503,28 +3521,28 @@
       <c r="Z55" s="8"/>
       <c r="AA55" s="8"/>
     </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:27">
       <c r="B56" s="9" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="8" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
       <c r="M56" s="8" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="N56" s="8"/>
       <c r="O56" s="8"/>
@@ -3532,12 +3550,12 @@
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
       <c r="S56" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="T56" s="8"/>
       <c r="U56" s="8"/>
       <c r="V56" s="8" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="W56" s="8"/>
       <c r="X56" s="8"/>
@@ -3545,7 +3563,7 @@
       <c r="Z56" s="8"/>
       <c r="AA56" s="8"/>
     </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:27">
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="8"/>
@@ -3573,7 +3591,7 @@
       <c r="Z57" s="8"/>
       <c r="AA57" s="8"/>
     </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:27">
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="8"/>
@@ -3601,7 +3619,7 @@
       <c r="Z58" s="8"/>
       <c r="AA58" s="8"/>
     </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:27">
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="8"/>
@@ -3629,7 +3647,7 @@
       <c r="Z59" s="8"/>
       <c r="AA59" s="8"/>
     </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:27">
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="8"/>
@@ -3657,7 +3675,7 @@
       <c r="Z60" s="8"/>
       <c r="AA60" s="8"/>
     </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:27">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="8"/>
@@ -3687,57 +3705,33 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="P50:R55"/>
-    <mergeCell ref="S50:U55"/>
-    <mergeCell ref="V50:X55"/>
-    <mergeCell ref="Y50:AA55"/>
-    <mergeCell ref="B50:C55"/>
-    <mergeCell ref="D50:F55"/>
-    <mergeCell ref="G50:I55"/>
-    <mergeCell ref="J50:L55"/>
-    <mergeCell ref="M50:O55"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B20:C25"/>
-    <mergeCell ref="D20:F25"/>
-    <mergeCell ref="G20:I25"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="D18:F19"/>
-    <mergeCell ref="G18:I19"/>
-    <mergeCell ref="J18:L19"/>
-    <mergeCell ref="J20:L25"/>
-    <mergeCell ref="M18:O19"/>
-    <mergeCell ref="M20:O25"/>
-    <mergeCell ref="P18:R19"/>
-    <mergeCell ref="P20:R25"/>
-    <mergeCell ref="V26:X31"/>
-    <mergeCell ref="S18:U19"/>
-    <mergeCell ref="V18:X19"/>
-    <mergeCell ref="Y18:AA19"/>
-    <mergeCell ref="S20:U25"/>
-    <mergeCell ref="V20:X25"/>
-    <mergeCell ref="Y20:AA25"/>
-    <mergeCell ref="Y26:AA31"/>
+    <mergeCell ref="P56:R61"/>
+    <mergeCell ref="S56:U61"/>
+    <mergeCell ref="V56:X61"/>
+    <mergeCell ref="Y56:AA61"/>
+    <mergeCell ref="B56:C61"/>
+    <mergeCell ref="D56:F61"/>
+    <mergeCell ref="G56:I61"/>
+    <mergeCell ref="J56:L61"/>
+    <mergeCell ref="M56:O61"/>
+    <mergeCell ref="V44:X49"/>
+    <mergeCell ref="Y44:AA49"/>
+    <mergeCell ref="S38:U43"/>
+    <mergeCell ref="V38:X43"/>
+    <mergeCell ref="Y38:AA43"/>
+    <mergeCell ref="P44:R49"/>
+    <mergeCell ref="S44:U49"/>
+    <mergeCell ref="B38:C43"/>
+    <mergeCell ref="D38:F43"/>
+    <mergeCell ref="G38:I43"/>
+    <mergeCell ref="J38:L43"/>
+    <mergeCell ref="M38:O43"/>
+    <mergeCell ref="P38:R43"/>
+    <mergeCell ref="B44:C49"/>
+    <mergeCell ref="D44:F49"/>
+    <mergeCell ref="G44:I49"/>
+    <mergeCell ref="J44:L49"/>
+    <mergeCell ref="M44:O49"/>
     <mergeCell ref="P32:R37"/>
     <mergeCell ref="S32:U37"/>
     <mergeCell ref="V32:X37"/>
@@ -3754,33 +3748,57 @@
     <mergeCell ref="J32:L37"/>
     <mergeCell ref="M32:O37"/>
     <mergeCell ref="S26:U31"/>
-    <mergeCell ref="P44:R49"/>
-    <mergeCell ref="S44:U49"/>
-    <mergeCell ref="B38:C43"/>
-    <mergeCell ref="D38:F43"/>
-    <mergeCell ref="G38:I43"/>
-    <mergeCell ref="J38:L43"/>
-    <mergeCell ref="M38:O43"/>
-    <mergeCell ref="P38:R43"/>
-    <mergeCell ref="B44:C49"/>
-    <mergeCell ref="D44:F49"/>
-    <mergeCell ref="G44:I49"/>
-    <mergeCell ref="J44:L49"/>
-    <mergeCell ref="M44:O49"/>
-    <mergeCell ref="V44:X49"/>
-    <mergeCell ref="Y44:AA49"/>
-    <mergeCell ref="S38:U43"/>
-    <mergeCell ref="V38:X43"/>
-    <mergeCell ref="Y38:AA43"/>
-    <mergeCell ref="P56:R61"/>
-    <mergeCell ref="S56:U61"/>
-    <mergeCell ref="V56:X61"/>
-    <mergeCell ref="Y56:AA61"/>
-    <mergeCell ref="B56:C61"/>
-    <mergeCell ref="D56:F61"/>
-    <mergeCell ref="G56:I61"/>
-    <mergeCell ref="J56:L61"/>
-    <mergeCell ref="M56:O61"/>
+    <mergeCell ref="V26:X31"/>
+    <mergeCell ref="S18:U19"/>
+    <mergeCell ref="V18:X19"/>
+    <mergeCell ref="Y18:AA19"/>
+    <mergeCell ref="S20:U25"/>
+    <mergeCell ref="V20:X25"/>
+    <mergeCell ref="Y20:AA25"/>
+    <mergeCell ref="Y26:AA31"/>
+    <mergeCell ref="J18:L19"/>
+    <mergeCell ref="J20:L25"/>
+    <mergeCell ref="M18:O19"/>
+    <mergeCell ref="M20:O25"/>
+    <mergeCell ref="P18:R19"/>
+    <mergeCell ref="P20:R25"/>
+    <mergeCell ref="B20:C25"/>
+    <mergeCell ref="D20:F25"/>
+    <mergeCell ref="G20:I25"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="D18:F19"/>
+    <mergeCell ref="G18:I19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="P50:R55"/>
+    <mergeCell ref="S50:U55"/>
+    <mergeCell ref="V50:X55"/>
+    <mergeCell ref="Y50:AA55"/>
+    <mergeCell ref="B50:C55"/>
+    <mergeCell ref="D50:F55"/>
+    <mergeCell ref="G50:I55"/>
+    <mergeCell ref="J50:L55"/>
+    <mergeCell ref="M50:O55"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3790,223 +3808,252 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C4:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" ht="22.5">
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" s="29">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="4">
+        <v>106</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" s="29">
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4">
+        <v>106</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7">
+      <c r="C7" s="29">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="4">
+        <v>106</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7">
+      <c r="C8" s="29">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
+        <v>106</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7">
+      <c r="C9" s="29">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="4">
+        <v>106</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7">
+      <c r="C10" s="29">
         <v>6</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="4">
+    <row r="11" spans="3:7">
+      <c r="C11" s="29">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="4">
+    <row r="12" spans="3:7">
+      <c r="C12" s="29">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
+    <row r="13" spans="3:7">
+      <c r="C13" s="29">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
+    <row r="14" spans="3:7">
+      <c r="C14" s="29">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7">
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7">
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="5"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="26" t="s">
-        <v>102</v>
+    <row r="22" spans="3:7">
+      <c r="C22" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="26"/>
+        <v>122</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="27"/>
       <c r="D23" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
+        <v>123</v>
+      </c>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>